<commit_message>
Working on tutorial 2
</commit_message>
<xml_diff>
--- a/pure4j-examples/src/test/resources/org/pure4j/examples/var_model/ConcordionVar.xlsx
+++ b/pure4j-examples/src/test/resources/org/pure4j/examples/var_model/ConcordionVar.xlsx
@@ -219,7 +219,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t>MSFT</t>
   </si>
@@ -335,6 +335,9 @@
     <t>Value At Risk:</t>
   </si>
   <si>
+    <t>Portfolio Pnl:</t>
+  </si>
+  <si>
     <t>Oct 11, 2015</t>
   </si>
   <si>
@@ -348,12 +351,6 @@
   </si>
   <si>
     <t>PnL per share will be:</t>
-  </si>
-  <si>
-    <t>Total Portfolio Pnl is:</t>
-  </si>
-  <si>
-    <t>USD</t>
   </si>
 </sst>
 </file>
@@ -482,7 +479,16 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="19">
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_-[$USD]\ * #,##0.00_-;\-[$USD]\ * #,##0.00_-;_-[$USD]\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_-[$USD]\ * #,##0.00_-;\-[$USD]\ * #,##0.00_-;_-[$USD]\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_-[$USD]\ * #,##0.00_-;\-[$USD]\ * #,##0.00_-;_-[$USD]\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="_-[$USD]\ * #,##0.00_-;\-[$USD]\ * #,##0.00_-;_-[$USD]\ * &quot;-&quot;??_-;_-@_-"/>
     </dxf>
@@ -590,15 +596,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="171" formatCode="[$USD]\ #,##0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="_-[$USD]\ * #,##0.00_-;\-[$USD]\ * #,##0.00_-;_-[$USD]\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="_-[$USD]\ * #,##0.00_-;\-[$USD]\ * #,##0.00_-;_-[$USD]\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="_-[$USD]\ * #,##0.00_-;\-[$USD]\ * #,##0.00_-;_-[$USD]\ * &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <font>
@@ -723,9 +720,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="167" formatCode="[$USD]\ #,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="_-[$USD]\ * #,##0.00_-;\-[$USD]\ * #,##0.00_-;_-[$USD]\ * &quot;-&quot;??_-;_-@_-"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -2798,32 +2792,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="G8:J28" totalsRowShown="0" dataDxfId="19" dataCellStyle="Currency">
-  <autoFilter ref="G8:J28"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="GOOG" dataDxfId="10" dataCellStyle="Currency">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="G8:I28" totalsRowShown="0" dataDxfId="3" dataCellStyle="Currency">
+  <autoFilter ref="G8:I28"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="GOOG" dataDxfId="2" dataCellStyle="Currency">
       <calculatedColumnFormula>Table4[[#This Row],[GOOG]]*C$4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="YAHOO" dataDxfId="9" dataCellStyle="Currency">
+    <tableColumn id="2" name="YAHOO" dataDxfId="1" dataCellStyle="Currency">
       <calculatedColumnFormula>Table4[[#This Row],[YHOO]]*C$5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="MSFT" dataDxfId="8" dataCellStyle="Currency">
+    <tableColumn id="3" name="MSFT" dataDxfId="0" dataCellStyle="Currency">
       <calculatedColumnFormula>Table4[[#This Row],[MSFT]]*C$6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Total Portfolio Pnl is:" dataDxfId="0" dataCellStyle="Currency"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="K8:K28" totalsRowShown="0" headerRowDxfId="18" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="K8:K28" totalsRowShown="0" headerRowDxfId="18" dataDxfId="9">
   <autoFilter ref="K8:K28"/>
   <sortState ref="K11:K30">
     <sortCondition ref="K10:K30"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" name="Portfolio" dataDxfId="7">
+    <tableColumn id="1" name="Portfolio" dataDxfId="10">
       <calculatedColumnFormula>SUM(Table5[#This Row])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2832,13 +2825,13 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B8:E28" totalsRowShown="0" dataDxfId="5" dataCellStyle="Percent">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B8:E28" totalsRowShown="0" dataDxfId="8" dataCellStyle="Percent">
   <autoFilter ref="B8:E28"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Date" dataDxfId="4"/>
-    <tableColumn id="2" name="GOOG" dataDxfId="3" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="YHOO" dataDxfId="2" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="MSFT" dataDxfId="1" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="Date" dataDxfId="7"/>
+    <tableColumn id="2" name="GOOG" dataDxfId="6" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="YHOO" dataDxfId="5" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="MSFT" dataDxfId="4" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3134,10 +3127,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B11" zoomScale="97" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="C7" zoomScale="97" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3165,10 +3158,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
         <v>40</v>
-      </c>
-      <c r="B3" t="s">
-        <v>39</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>27</v>
@@ -3200,7 +3193,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
         <v>30</v>
@@ -3215,7 +3208,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G8" t="s">
         <v>1</v>
@@ -3227,7 +3220,7 @@
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="K8" s="8" t="s">
         <v>26</v>
@@ -3258,7 +3251,6 @@
         <f>Table4[[#This Row],[MSFT]]*C$6</f>
         <v>0.86908284023667903</v>
       </c>
-      <c r="J9" s="7"/>
       <c r="K9" s="13">
         <f>SUM(Table5[#This Row])</f>
         <v>-1.7986170072902263</v>
@@ -3289,7 +3281,6 @@
         <f>Table4[[#This Row],[MSFT]]*C$6</f>
         <v>-0.75243163883281783</v>
       </c>
-      <c r="J10" s="7"/>
       <c r="K10" s="13">
         <f>SUM(Table5[#This Row])</f>
         <v>-0.70258829599355588</v>
@@ -3320,7 +3311,6 @@
         <f>Table4[[#This Row],[MSFT]]*C$6</f>
         <v>0.57216685123662181</v>
       </c>
-      <c r="J11" s="7"/>
       <c r="K11" s="13">
         <f>SUM(Table5[#This Row])</f>
         <v>1.9793924887566927</v>
@@ -3351,7 +3341,6 @@
         <f>Table4[[#This Row],[MSFT]]*C$6</f>
         <v>2.3616096731532199</v>
       </c>
-      <c r="J12" s="7"/>
       <c r="K12" s="13">
         <f>SUM(Table5[#This Row])</f>
         <v>2.058725333087208</v>
@@ -3382,7 +3371,6 @@
         <f>Table4[[#This Row],[MSFT]]*C$6</f>
         <v>0.15137180700093289</v>
       </c>
-      <c r="J13" s="7"/>
       <c r="K13" s="13">
         <f>SUM(Table5[#This Row])</f>
         <v>0.37410117227305584</v>
@@ -3413,7 +3401,6 @@
         <f>Table4[[#This Row],[MSFT]]*C$6</f>
         <v>-0.88147036759189668</v>
       </c>
-      <c r="J14" s="7"/>
       <c r="K14" s="13">
         <f>SUM(Table5[#This Row])</f>
         <v>-0.62330790992989327</v>
@@ -3444,7 +3431,6 @@
         <f>Table4[[#This Row],[MSFT]]*C$6</f>
         <v>-0.41090773253641411</v>
       </c>
-      <c r="J15" s="7"/>
       <c r="K15" s="13">
         <f>SUM(Table5[#This Row])</f>
         <v>1.0994981643436819</v>
@@ -3475,13 +3461,12 @@
         <f>Table4[[#This Row],[MSFT]]*C$6</f>
         <v>0</v>
       </c>
-      <c r="J16" s="7"/>
       <c r="K16" s="13">
         <f>SUM(Table5[#This Row])</f>
         <v>2.1099718033805059</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="11">
         <v>42305</v>
       </c>
@@ -3506,13 +3491,12 @@
         <f>Table4[[#This Row],[MSFT]]*C$6</f>
         <v>-0.83348768290424369</v>
       </c>
-      <c r="J17" s="7"/>
       <c r="K17" s="13">
         <f>SUM(Table5[#This Row])</f>
         <v>-2.756483957816025</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="11">
         <v>42304</v>
       </c>
@@ -3537,13 +3521,12 @@
         <f>Table4[[#This Row],[MSFT]]*C$6</f>
         <v>2.7793641728536045</v>
       </c>
-      <c r="J18" s="7"/>
       <c r="K18" s="13">
         <f>SUM(Table5[#This Row])</f>
         <v>9.1642598663896013</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="11">
         <v>42303</v>
       </c>
@@ -3568,13 +3551,12 @@
         <f>Table4[[#This Row],[MSFT]]*C$6</f>
         <v>0.43977055449331282</v>
       </c>
-      <c r="J19" s="7"/>
       <c r="K19" s="13">
         <f>SUM(Table5[#This Row])</f>
         <v>-1.6571019293639133</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" s="11">
         <v>42300</v>
       </c>
@@ -3599,13 +3581,12 @@
         <f>Table4[[#This Row],[MSFT]]*C$6</f>
         <v>10.035766884073215</v>
       </c>
-      <c r="J20" s="7"/>
       <c r="K20" s="13">
         <f>SUM(Table5[#This Row])</f>
         <v>26.976545309231057</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="11">
         <v>42299</v>
       </c>
@@ -3630,13 +3611,12 @@
         <f>Table4[[#This Row],[MSFT]]*C$6</f>
         <v>-0.81385642737896724</v>
       </c>
-      <c r="J21" s="7"/>
       <c r="K21" s="13">
         <f>SUM(Table5[#This Row])</f>
         <v>-4.4480602192926604</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="11">
         <v>42298</v>
       </c>
@@ -3661,13 +3641,12 @@
         <f>Table4[[#This Row],[MSFT]]*C$6</f>
         <v>1.0118043844856706</v>
       </c>
-      <c r="J22" s="7"/>
       <c r="K22" s="13">
         <f>SUM(Table5[#This Row])</f>
         <v>-4.7474950486520404</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" s="11">
         <v>42297</v>
       </c>
@@ -3692,13 +3671,12 @@
         <f>Table4[[#This Row],[MSFT]]*C$6</f>
         <v>4.2176296921114798E-2</v>
       </c>
-      <c r="J23" s="7"/>
       <c r="K23" s="13">
         <f>SUM(Table5[#This Row])</f>
         <v>1.1662576124255475</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" s="11">
         <v>42296</v>
       </c>
@@ -3723,13 +3701,12 @@
         <f>Table4[[#This Row],[MSFT]]*C$6</f>
         <v>0.85070182900892632</v>
       </c>
-      <c r="J24" s="7"/>
       <c r="K24" s="13">
         <f>SUM(Table5[#This Row])</f>
         <v>-0.72009775218878636</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" s="11">
         <v>42293</v>
       </c>
@@ -3754,13 +3731,12 @@
         <f>Table4[[#This Row],[MSFT]]*C$6</f>
         <v>2.1272069772404478E-2</v>
       </c>
-      <c r="J25" s="7"/>
       <c r="K25" s="13">
         <f>SUM(Table5[#This Row])</f>
         <v>5.2278786495863816</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="11">
         <v>42292</v>
       </c>
@@ -3785,13 +3761,12 @@
         <f>Table4[[#This Row],[MSFT]]*C$6</f>
         <v>0.77170418006431429</v>
       </c>
-      <c r="J26" s="7"/>
       <c r="K26" s="13">
         <f>SUM(Table5[#This Row])</f>
         <v>1.4273899406358703</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B27" s="11">
         <v>42291</v>
       </c>
@@ -3816,13 +3791,12 @@
         <f>Table4[[#This Row],[MSFT]]*C$6</f>
         <v>0.19329896907216426</v>
       </c>
-      <c r="J27" s="7"/>
       <c r="K27" s="13">
         <f>SUM(Table5[#This Row])</f>
         <v>0.89752442879790229</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B28" s="11">
         <v>42290</v>
       </c>
@@ -3847,13 +3821,12 @@
         <f>Table4[[#This Row],[MSFT]]*C$6</f>
         <v>-0.89399744572157269</v>
       </c>
-      <c r="J28" s="7"/>
       <c r="K28" s="13">
         <f>SUM(Table5[#This Row])</f>
         <v>-1.1874869135530042</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B29" s="11"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -3863,16 +3836,13 @@
       <c r="I29" s="7"/>
       <c r="K29" s="10"/>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
       <c r="J31" s="9" t="s">
         <v>37</v>
       </c>
       <c r="K31" s="15">
         <f>SMALL(Table6[Portfolio], 20-C1*20)</f>
         <v>-4.4480602192926604</v>
-      </c>
-      <c r="L31" s="9" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -4910,7 +4880,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B25" s="1">
         <v>645.32000000000005</v>

</xml_diff>